<commit_message>
recalculate age and create new df which is age of each player for each season from 2015-2020
</commit_message>
<xml_diff>
--- a/Summary2015-2020_PO.xlsx
+++ b/Summary2015-2020_PO.xlsx
@@ -1,7 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
@@ -9,16 +12,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1" mc:Ignorable="x14ac">
+  <numFmts count="9">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -32,18 +43,28 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,11 +395,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="8.53" customWidth="1"/>
+    <col min="2" max="2" width="13.38" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">

</xml_diff>